<commit_message>
Added code to plot  pH profile curves and profile collection sorted by pH
</commit_message>
<xml_diff>
--- a/Perfiles_AQP/Data/horizontes.xlsx
+++ b/Perfiles_AQP/Data/horizontes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VALENTINA\Documents\SERVICIO GOLÓGICO COLOMBIANO\SUELOS\suelos3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmguio\Documents\2024_SGC_SUEREC\PROYECTOS DE CODIGO\SGC_SUEREC\Perfiles_AQP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22AC8EB-A965-4DE1-B49C-73216440625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79CF7CF-2BFC-41BD-9926-DD7253645CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3142D5B3-B4B5-461D-AC03-E58BB097A201}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3142D5B3-B4B5-461D-AC03-E58BB097A201}"/>
   </bookViews>
   <sheets>
     <sheet name="ejemplo_tabla_horizontes" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="126">
   <si>
     <t>id</t>
   </si>
@@ -158,34 +159,259 @@
     <t>distinctness</t>
   </si>
   <si>
-    <t>Gradual</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>Diffuse</t>
-  </si>
-  <si>
-    <t>Abrupt</t>
-  </si>
-  <si>
-    <t>Smooth</t>
-  </si>
-  <si>
-    <t>Wavy</t>
-  </si>
-  <si>
-    <t>Irregular</t>
-  </si>
-  <si>
-    <t>Bkoken</t>
-  </si>
-  <si>
     <t>topography</t>
+  </si>
+  <si>
+    <t>ph_lab</t>
+  </si>
+  <si>
+    <t>ph_t_lab</t>
+  </si>
+  <si>
+    <t>5.16</t>
+  </si>
+  <si>
+    <t>5.26</t>
+  </si>
+  <si>
+    <t>5.36</t>
+  </si>
+  <si>
+    <t>5.66</t>
+  </si>
+  <si>
+    <t>5.71</t>
+  </si>
+  <si>
+    <t>5.67</t>
+  </si>
+  <si>
+    <t>5.47</t>
+  </si>
+  <si>
+    <t>id_campo</t>
+  </si>
+  <si>
+    <t>6.23</t>
+  </si>
+  <si>
+    <t>6.34</t>
+  </si>
+  <si>
+    <t>5.90</t>
+  </si>
+  <si>
+    <t>5.40</t>
+  </si>
+  <si>
+    <t>5.55</t>
+  </si>
+  <si>
+    <t>6.47</t>
+  </si>
+  <si>
+    <t>5.93</t>
+  </si>
+  <si>
+    <t>5.80</t>
+  </si>
+  <si>
+    <t>5.64</t>
+  </si>
+  <si>
+    <t>5.82</t>
+  </si>
+  <si>
+    <t>5.27</t>
+  </si>
+  <si>
+    <t>5.25</t>
+  </si>
+  <si>
+    <t>5.13</t>
+  </si>
+  <si>
+    <t>5.53</t>
+  </si>
+  <si>
+    <t>5.09</t>
+  </si>
+  <si>
+    <t>24.8</t>
+  </si>
+  <si>
+    <t>24.5</t>
+  </si>
+  <si>
+    <t>23.9</t>
+  </si>
+  <si>
+    <t>24.6</t>
+  </si>
+  <si>
+    <t>24.9</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>24.7</t>
+  </si>
+  <si>
+    <t>23.2</t>
+  </si>
+  <si>
+    <t>24.3</t>
+  </si>
+  <si>
+    <t>24.4</t>
+  </si>
+  <si>
+    <t>4.60</t>
+  </si>
+  <si>
+    <t>5.95</t>
+  </si>
+  <si>
+    <t>5.42</t>
+  </si>
+  <si>
+    <t>4.92</t>
+  </si>
+  <si>
+    <t>4.61</t>
+  </si>
+  <si>
+    <t>5.77</t>
+  </si>
+  <si>
+    <t>5.86</t>
+  </si>
+  <si>
+    <t>5.63</t>
+  </si>
+  <si>
+    <t>4.82</t>
+  </si>
+  <si>
+    <t>5.31</t>
+  </si>
+  <si>
+    <t>5.21</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>4.94</t>
+  </si>
+  <si>
+    <t>5.22</t>
+  </si>
+  <si>
+    <t>4.59</t>
+  </si>
+  <si>
+    <t>5.89</t>
+  </si>
+  <si>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t>24.1</t>
+  </si>
+  <si>
+    <t>23.7</t>
+  </si>
+  <si>
+    <t>24.2</t>
+  </si>
+  <si>
+    <t>23.6</t>
+  </si>
+  <si>
+    <t>25.1</t>
+  </si>
+  <si>
+    <t>6.04</t>
+  </si>
+  <si>
+    <t>5.96</t>
+  </si>
+  <si>
+    <t>6.24</t>
+  </si>
+  <si>
+    <t>6.07</t>
+  </si>
+  <si>
+    <t>4.91</t>
+  </si>
+  <si>
+    <t>4.38</t>
+  </si>
+  <si>
+    <t>4.66</t>
+  </si>
+  <si>
+    <t>5.94</t>
+  </si>
+  <si>
+    <t>5.81</t>
+  </si>
+  <si>
+    <t>5.78</t>
+  </si>
+  <si>
+    <t>23.4</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
+    <t>23.5</t>
+  </si>
+  <si>
+    <t>5.58</t>
+  </si>
+  <si>
+    <t>5.88</t>
+  </si>
+  <si>
+    <t>5.87</t>
+  </si>
+  <si>
+    <t>5.74</t>
+  </si>
+  <si>
+    <t>5.48</t>
+  </si>
+  <si>
+    <t>5.65</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>gradual</t>
+  </si>
+  <si>
+    <t>diffuse</t>
+  </si>
+  <si>
+    <t>abrupt</t>
+  </si>
+  <si>
+    <t>broken</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>wavy</t>
+  </si>
+  <si>
+    <t>irregular</t>
   </si>
 </sst>
 </file>
@@ -687,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -705,6 +931,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1080,15 +1307,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D627FE3-B1D1-4785-B94C-0D0D8B8F39DD}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="15" max="16" width="10.90625" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1126,10 +1359,16 @@
         <v>40</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>970021</v>
       </c>
@@ -1167,13 +1406,19 @@
         <v>10</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O2" s="7">
+        <v>5.16</v>
+      </c>
+      <c r="P2" s="7">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>970022</v>
       </c>
@@ -1211,13 +1456,19 @@
         <v>60</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O3" s="7">
+        <v>5.71</v>
+      </c>
+      <c r="P3" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>970023</v>
       </c>
@@ -1255,13 +1506,19 @@
         <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O4" s="7">
+        <v>5.67</v>
+      </c>
+      <c r="P4" s="7">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>970024</v>
       </c>
@@ -1298,14 +1555,16 @@
       <c r="L5" s="3">
         <v>60</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M5" s="1"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="7">
+        <v>5.66</v>
+      </c>
+      <c r="P5" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>970025</v>
       </c>
@@ -1343,13 +1602,13 @@
         <v>10</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>970026</v>
       </c>
@@ -1386,14 +1645,16 @@
       <c r="L7" s="3">
         <v>60</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M7" s="1"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="7">
+        <v>6.23</v>
+      </c>
+      <c r="P7" s="7">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>970027</v>
       </c>
@@ -1431,13 +1692,19 @@
         <v>15</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O8" s="7">
+        <v>6.34</v>
+      </c>
+      <c r="P8" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>970028</v>
       </c>
@@ -1475,13 +1742,19 @@
         <v>10</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O9" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="P9" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>970029</v>
       </c>
@@ -1519,13 +1792,19 @@
         <v>10</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O10" s="7">
+        <v>5.4</v>
+      </c>
+      <c r="P10" s="7">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>970030</v>
       </c>
@@ -1563,13 +1842,19 @@
         <v>15</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O11" s="7">
+        <v>5.55</v>
+      </c>
+      <c r="P11" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>970031</v>
       </c>
@@ -1607,13 +1892,19 @@
         <v>10</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O12" s="7">
+        <v>6.47</v>
+      </c>
+      <c r="P12" s="7">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>970032</v>
       </c>
@@ -1651,13 +1942,19 @@
         <v>10</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O13" s="7">
+        <v>5.93</v>
+      </c>
+      <c r="P13" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>970033</v>
       </c>
@@ -1695,13 +1992,19 @@
         <v>60</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O14" s="7">
+        <v>6.23</v>
+      </c>
+      <c r="P14" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>970034</v>
       </c>
@@ -1739,13 +2042,19 @@
         <v>60</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O15" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="P15" s="7">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>970035</v>
       </c>
@@ -1782,14 +2091,16 @@
       <c r="L16" s="3">
         <v>60</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M16" s="1"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="7">
+        <v>5.67</v>
+      </c>
+      <c r="P16" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>970036</v>
       </c>
@@ -1826,14 +2137,16 @@
       <c r="L17" s="3">
         <v>15</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M17" s="1"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="7">
+        <v>5.64</v>
+      </c>
+      <c r="P17" s="7">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>970037</v>
       </c>
@@ -1871,13 +2184,19 @@
         <v>10</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O18" s="7">
+        <v>5.82</v>
+      </c>
+      <c r="P18" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>970038</v>
       </c>
@@ -1915,13 +2234,19 @@
         <v>10</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O19" s="7">
+        <v>5.27</v>
+      </c>
+      <c r="P19" s="7">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>970039</v>
       </c>
@@ -1959,13 +2284,19 @@
         <v>10</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O20" s="7">
+        <v>5.25</v>
+      </c>
+      <c r="P20" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>970040</v>
       </c>
@@ -2002,14 +2333,16 @@
       <c r="L21" s="3">
         <v>10</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M21" s="1"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="7">
+        <v>5.13</v>
+      </c>
+      <c r="P21" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>970041</v>
       </c>
@@ -2047,13 +2380,19 @@
         <v>10</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O22" s="7">
+        <v>5.53</v>
+      </c>
+      <c r="P22" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>970042</v>
       </c>
@@ -2091,13 +2430,19 @@
         <v>10</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O23" s="7">
+        <v>5.09</v>
+      </c>
+      <c r="P23" s="7">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>970043</v>
       </c>
@@ -2135,13 +2480,19 @@
         <v>10</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O24" s="7">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P24" s="7">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>970044</v>
       </c>
@@ -2178,14 +2529,16 @@
       <c r="L25" s="3">
         <v>60</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M25" s="1"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="7">
+        <v>5.95</v>
+      </c>
+      <c r="P25" s="7">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>970045</v>
       </c>
@@ -2223,13 +2576,19 @@
         <v>10</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O26" s="7">
+        <v>5.27</v>
+      </c>
+      <c r="P26" s="7">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>970046</v>
       </c>
@@ -2267,13 +2626,19 @@
         <v>10</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O27" s="7">
+        <v>5.42</v>
+      </c>
+      <c r="P27" s="7">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>970047</v>
       </c>
@@ -2310,14 +2675,16 @@
       <c r="L28" s="3">
         <v>10</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N28" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M28" s="1"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="7">
+        <v>4.92</v>
+      </c>
+      <c r="P28" s="7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>970048</v>
       </c>
@@ -2355,13 +2722,19 @@
         <v>10</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O29" s="7">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="P29" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>970049</v>
       </c>
@@ -2399,13 +2772,19 @@
         <v>10</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N30" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O30" s="7">
+        <v>5.77</v>
+      </c>
+      <c r="P30" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>970050</v>
       </c>
@@ -2443,13 +2822,19 @@
         <v>15</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O31" s="7">
+        <v>5.86</v>
+      </c>
+      <c r="P31" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>970051</v>
       </c>
@@ -2487,13 +2872,19 @@
         <v>60</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O32" s="7">
+        <v>5.63</v>
+      </c>
+      <c r="P32" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>970052</v>
       </c>
@@ -2531,13 +2922,19 @@
         <v>10</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O33" s="7">
+        <v>4.92</v>
+      </c>
+      <c r="P33" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>970053</v>
       </c>
@@ -2574,14 +2971,16 @@
       <c r="L34" s="3">
         <v>60</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M34" s="1"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="7">
+        <v>4.82</v>
+      </c>
+      <c r="P34" s="7">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>970054</v>
       </c>
@@ -2619,13 +3018,19 @@
         <v>10</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O35" s="7">
+        <v>5.47</v>
+      </c>
+      <c r="P35" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>970055</v>
       </c>
@@ -2663,13 +3068,19 @@
         <v>10</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O36" s="7">
+        <v>5.31</v>
+      </c>
+      <c r="P36" s="7">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>970056</v>
       </c>
@@ -2707,13 +3118,19 @@
         <v>10</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O37" s="7">
+        <v>5.31</v>
+      </c>
+      <c r="P37" s="7">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>970057</v>
       </c>
@@ -2750,14 +3167,16 @@
       <c r="L38" s="3">
         <v>30</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M38" s="1"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="7">
+        <v>5.21</v>
+      </c>
+      <c r="P38" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>970058</v>
       </c>
@@ -2795,13 +3214,19 @@
         <v>15</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O39" s="7">
+        <v>5.8</v>
+      </c>
+      <c r="P39" s="7">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>970059</v>
       </c>
@@ -2839,13 +3264,19 @@
         <v>10</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O40" s="7">
+        <v>5.14</v>
+      </c>
+      <c r="P40" s="7">
+        <v>25.1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>970060</v>
       </c>
@@ -2883,13 +3314,19 @@
         <v>10</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O41" s="7">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="P41" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>970061</v>
       </c>
@@ -2926,14 +3363,16 @@
       <c r="L42" s="3">
         <v>60</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M42" s="1"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="7">
+        <v>5.21</v>
+      </c>
+      <c r="P42" s="7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>970062</v>
       </c>
@@ -2971,13 +3410,19 @@
         <v>30</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N43" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O43" s="7">
+        <v>5.26</v>
+      </c>
+      <c r="P43" s="7">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>970063</v>
       </c>
@@ -3015,13 +3460,19 @@
         <v>15</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N44" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O44" s="7">
+        <v>5.22</v>
+      </c>
+      <c r="P44" s="7">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>970064</v>
       </c>
@@ -3059,13 +3510,19 @@
         <v>10</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O45" s="7">
+        <v>4.59</v>
+      </c>
+      <c r="P45" s="7">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>970065</v>
       </c>
@@ -3102,14 +3559,16 @@
       <c r="L46" s="3">
         <v>10</v>
       </c>
-      <c r="M46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M46" s="1"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="7">
+        <v>5.89</v>
+      </c>
+      <c r="P46" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>970066</v>
       </c>
@@ -3147,13 +3606,19 @@
         <v>10</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O47" s="7">
+        <v>5.75</v>
+      </c>
+      <c r="P47" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>970067</v>
       </c>
@@ -3191,13 +3656,19 @@
         <v>10</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O48" s="7">
+        <v>6.04</v>
+      </c>
+      <c r="P48" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>970068</v>
       </c>
@@ -3235,13 +3706,19 @@
         <v>15</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O49" s="7">
+        <v>5.25</v>
+      </c>
+      <c r="P49" s="7">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>970069</v>
       </c>
@@ -3279,13 +3756,19 @@
         <v>10</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N50" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O50" s="7">
+        <v>4.92</v>
+      </c>
+      <c r="P50" s="7">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>970070</v>
       </c>
@@ -3322,14 +3805,16 @@
       <c r="L51" s="3">
         <v>60</v>
       </c>
-      <c r="M51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M51" s="1"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="7">
+        <v>5.96</v>
+      </c>
+      <c r="P51" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>970071</v>
       </c>
@@ -3367,13 +3852,19 @@
         <v>15</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O52" s="7">
+        <v>6.24</v>
+      </c>
+      <c r="P52" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>970072</v>
       </c>
@@ -3411,13 +3902,19 @@
         <v>10</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N53" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O53" s="7">
+        <v>6.07</v>
+      </c>
+      <c r="P53" s="7">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>970073</v>
       </c>
@@ -3455,13 +3952,19 @@
         <v>10</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O54" s="7">
+        <v>4.91</v>
+      </c>
+      <c r="P54" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>970074</v>
       </c>
@@ -3498,14 +4001,16 @@
       <c r="L55" s="3">
         <v>10</v>
       </c>
-      <c r="M55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M55" s="1"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="7">
+        <v>5.36</v>
+      </c>
+      <c r="P55" s="7">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>970075</v>
       </c>
@@ -3543,13 +4048,13 @@
         <v>15</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>970076</v>
       </c>
@@ -3587,13 +4092,19 @@
         <v>10</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O57" s="7">
+        <v>4.38</v>
+      </c>
+      <c r="P57" s="7">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>970077</v>
       </c>
@@ -3631,13 +4142,19 @@
         <v>10</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O58" s="7">
+        <v>5.42</v>
+      </c>
+      <c r="P58" s="7">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>970079</v>
       </c>
@@ -3675,13 +4192,19 @@
         <v>10</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N59" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O59" s="7">
+        <v>4.66</v>
+      </c>
+      <c r="P59" s="7">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>970080</v>
       </c>
@@ -3718,14 +4241,16 @@
       <c r="L60" s="3">
         <v>10</v>
       </c>
-      <c r="M60" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N60" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M60" s="1"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="7">
+        <v>5.96</v>
+      </c>
+      <c r="P60" s="7">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>970081</v>
       </c>
@@ -3763,13 +4288,19 @@
         <v>10</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O61" s="7">
+        <v>5.94</v>
+      </c>
+      <c r="P61" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>970082</v>
       </c>
@@ -3807,13 +4338,19 @@
         <v>10</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N62" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O62" s="7">
+        <v>5.81</v>
+      </c>
+      <c r="P62" s="7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>970083</v>
       </c>
@@ -3851,13 +4388,19 @@
         <v>15</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="O63" s="7">
+        <v>5.78</v>
+      </c>
+      <c r="P63" s="7">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>970084</v>
       </c>
@@ -3895,13 +4438,13 @@
         <v>10</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N64" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>970085</v>
       </c>
@@ -3939,13 +4482,13 @@
         <v>10</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>970086</v>
       </c>
@@ -3983,13 +4526,19 @@
         <v>10</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N66" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="O66" s="7">
+        <v>5.58</v>
+      </c>
+      <c r="P66" s="7">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>970087</v>
       </c>
@@ -4026,14 +4575,16 @@
       <c r="L67" s="3">
         <v>10</v>
       </c>
-      <c r="M67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N67" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M67" s="1"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="7">
+        <v>5.88</v>
+      </c>
+      <c r="P67" s="7">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>970088</v>
       </c>
@@ -4071,13 +4622,13 @@
         <v>10</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N68" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>970089</v>
       </c>
@@ -4115,13 +4666,13 @@
         <v>10</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N69" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>970090</v>
       </c>
@@ -4159,13 +4710,13 @@
         <v>10</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N70" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>970091</v>
       </c>
@@ -4202,14 +4753,10 @@
       <c r="L71" s="3">
         <v>10</v>
       </c>
-      <c r="M71" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N71" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M71" s="1"/>
+      <c r="N71" s="5"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>970092</v>
       </c>
@@ -4244,13 +4791,13 @@
         <v>10</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N72" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>970093</v>
       </c>
@@ -4285,13 +4832,13 @@
         <v>60</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N73" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>970094</v>
       </c>
@@ -4326,13 +4873,13 @@
         <v>10</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N74" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>970095</v>
       </c>
@@ -4366,14 +4913,10 @@
       <c r="L75" s="3">
         <v>10</v>
       </c>
-      <c r="M75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N75" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M75" s="1"/>
+      <c r="N75" s="5"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>970096</v>
       </c>
@@ -4408,13 +4951,19 @@
         <v>10</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N76" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="O76" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="P76" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>970097</v>
       </c>
@@ -4449,13 +4998,13 @@
         <v>10</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N77" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>970098</v>
       </c>
@@ -4489,14 +5038,10 @@
       <c r="L78" s="3">
         <v>10</v>
       </c>
-      <c r="M78" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N78" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M78" s="1"/>
+      <c r="N78" s="5"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>970099</v>
       </c>
@@ -4531,13 +5076,13 @@
         <v>10</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N79" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>970100</v>
       </c>
@@ -4572,13 +5117,13 @@
         <v>60</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N80" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>970101</v>
       </c>
@@ -4613,13 +5158,13 @@
         <v>60</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N81" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>970102</v>
       </c>
@@ -4654,13 +5199,13 @@
         <v>10</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N82" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>970103</v>
       </c>
@@ -4694,14 +5239,16 @@
       <c r="L83" s="3">
         <v>10</v>
       </c>
-      <c r="M83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N83" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M83" s="1"/>
+      <c r="N83" s="5"/>
+      <c r="O83" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="P83" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>970104</v>
       </c>
@@ -4736,13 +5283,13 @@
         <v>10</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="N84" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>970105</v>
       </c>
@@ -4777,13 +5324,13 @@
         <v>10</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N85" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>970106</v>
       </c>
@@ -4817,14 +5364,10 @@
       <c r="L86" s="3">
         <v>10</v>
       </c>
-      <c r="M86" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N86" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M86" s="1"/>
+      <c r="N86" s="5"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>970107</v>
       </c>
@@ -4859,13 +5402,19 @@
         <v>60</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="N87" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="O87" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="P87" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>970108</v>
       </c>
@@ -4900,13 +5449,19 @@
         <v>10</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="N88" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O88" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P88" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>970109</v>
       </c>
@@ -4941,13 +5496,19 @@
         <v>30</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="N89" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="O89" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="P89" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>970110</v>
       </c>
@@ -4981,11 +5542,665 @@
       <c r="L90" s="3">
         <v>60</v>
       </c>
-      <c r="M90" s="1" t="s">
+      <c r="M90" s="1"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="P90" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{110D7199-A7C2-4227-96BC-37411CC07C12}">
+  <dimension ref="A1:B90"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N90" s="5" t="s">
-        <v>42</v>
+      <c r="B1" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizacion de datos de horizontes
</commit_message>
<xml_diff>
--- a/Perfiles_AQP/Data/horizontes.xlsx
+++ b/Perfiles_AQP/Data/horizontes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmguio\Documents\2024_SGC_SUEREC\PROYECTOS DE CODIGO\SGC_SUEREC\Perfiles_AQP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79CF7CF-2BFC-41BD-9926-DD7253645CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2523B4BA-4B87-47EE-BDA3-828D1F689911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{3142D5B3-B4B5-461D-AC03-E58BB097A201}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="126">
   <si>
     <t>id</t>
   </si>
@@ -913,7 +913,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,6 +932,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1309,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D627FE3-B1D1-4785-B94C-0D0D8B8F39DD}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q84" sqref="Q84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4053,6 +4054,9 @@
       <c r="N56" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O56" s="7">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
@@ -4443,6 +4447,9 @@
       <c r="N64" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O64" s="7">
+        <v>5.3</v>
+      </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
@@ -4486,6 +4493,9 @@
       </c>
       <c r="N65" s="5" t="s">
         <v>125</v>
+      </c>
+      <c r="O65" s="7">
+        <v>5.8</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.35">
@@ -4627,6 +4637,9 @@
       <c r="N68" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O68" s="8">
+        <v>5.88</v>
+      </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
@@ -4671,6 +4684,9 @@
       <c r="N69" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O69" s="8">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
@@ -4715,6 +4731,9 @@
       <c r="N70" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O70" s="8">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
@@ -4755,6 +4774,9 @@
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="5"/>
+      <c r="O71" s="8">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
@@ -4796,6 +4818,9 @@
       <c r="N72" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O72" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
@@ -4837,6 +4862,9 @@
       <c r="N73" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O73" s="8">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
@@ -4878,6 +4906,9 @@
       <c r="N74" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O74" s="8">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
@@ -4915,6 +4946,9 @@
       </c>
       <c r="M75" s="1"/>
       <c r="N75" s="5"/>
+      <c r="O75" s="8">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
@@ -4956,8 +4990,8 @@
       <c r="N76" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O76" s="7" t="s">
-        <v>114</v>
+      <c r="O76" s="8">
+        <v>5.87</v>
       </c>
       <c r="P76" s="7" t="s">
         <v>70</v>
@@ -5003,6 +5037,9 @@
       <c r="N77" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O77" s="8">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
@@ -5040,6 +5077,9 @@
       </c>
       <c r="M78" s="1"/>
       <c r="N78" s="5"/>
+      <c r="O78" s="8">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
@@ -5081,6 +5121,9 @@
       <c r="N79" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O79" s="8">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
@@ -5122,6 +5165,9 @@
       <c r="N80" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O80" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
@@ -5163,6 +5209,9 @@
       <c r="N81" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O81" s="8">
+        <v>5.7</v>
+      </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
@@ -5204,6 +5253,9 @@
       <c r="N82" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O82" s="8">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
@@ -5241,8 +5293,8 @@
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="5"/>
-      <c r="O83" s="7" t="s">
-        <v>115</v>
+      <c r="O83" s="8">
+        <v>5.74</v>
       </c>
       <c r="P83" s="7" t="s">
         <v>95</v>
@@ -5288,6 +5340,9 @@
       <c r="N84" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="O84" s="8">
+        <v>5.0999999999999996</v>
+      </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
@@ -5329,6 +5384,9 @@
       <c r="N85" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="O85" s="8">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
@@ -5366,6 +5424,9 @@
       </c>
       <c r="M86" s="1"/>
       <c r="N86" s="5"/>
+      <c r="O86" s="8">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
@@ -5407,8 +5468,8 @@
       <c r="N87" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O87" s="7" t="s">
-        <v>79</v>
+      <c r="O87" s="8">
+        <v>5.42</v>
       </c>
       <c r="P87" s="7" t="s">
         <v>94</v>
@@ -5454,8 +5515,8 @@
       <c r="N88" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="O88" s="7" t="s">
-        <v>55</v>
+      <c r="O88" s="8">
+        <v>5.4</v>
       </c>
       <c r="P88" s="7" t="s">
         <v>110</v>
@@ -5501,8 +5562,8 @@
       <c r="N89" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="O89" s="7" t="s">
-        <v>116</v>
+      <c r="O89" s="8">
+        <v>5.48</v>
       </c>
       <c r="P89" s="7" t="s">
         <v>72</v>
@@ -5544,8 +5605,8 @@
       </c>
       <c r="M90" s="1"/>
       <c r="N90" s="5"/>
-      <c r="O90" s="7" t="s">
-        <v>117</v>
+      <c r="O90" s="8">
+        <v>5.65</v>
       </c>
       <c r="P90" s="7" t="s">
         <v>75</v>

</xml_diff>